<commit_message>
cleaned up naming conventions, added new errors, added to to-do list, changed timer time
</commit_message>
<xml_diff>
--- a/twitter bot errors.xlsx
+++ b/twitter bot errors.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>code': 108, 'message': 'Cannot find specified user.</t>
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>'message': 'You have already favorited this status.', 'code': 139}</t>
   </si>
 </sst>
 </file>
@@ -347,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -365,6 +368,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
simplified fav/follow keyword list stuff, also added errors
</commit_message>
<xml_diff>
--- a/twitter bot errors.xlsx
+++ b/twitter bot errors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>code': 108, 'message': 'Cannot find specified user.</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>'message': 'You have already favorited this status.', 'code': 139}</t>
+  </si>
+  <si>
+    <t>code': 139, 'message': 'You have already favorited this status.'</t>
   </si>
 </sst>
 </file>
@@ -350,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -373,6 +376,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added to to-do list, added other mentioed user examples.txt and known bot-spotters.xlx, also added errors
</commit_message>
<xml_diff>
--- a/twitter bot errors.xlsx
+++ b/twitter bot errors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>code': 108, 'message': 'Cannot find specified user.</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>code': 139, 'message': 'You have already favorited this status.'</t>
+  </si>
+  <si>
+    <t>UnicodeEncodeError: 'charmap' codec can't encode character '\u2026' in position 130: character maps to &lt;undefined&gt;</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,6 +384,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>